<commit_message>
Updated paramsheet.py and hsdmix.py
paramsheet.py
- converts Qm from meq/g to meq/kg
- converts Qf from meq/ml to meq/L
- calculates Q from Qm or Qf
- adds Q to the parameters data

hsdmix.py
- accept Q as a parameter
- ignores Qm and RHOP

reg_test_input.xlsx
- includes Qf as an alternative to Qm
</commit_message>
<xml_diff>
--- a/IonExchangeModel/test/data/reg_test_input_alt.xlsx
+++ b/IonExchangeModel/test/data/reg_test_input_alt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LHaupert\Repos\GitHub\Water_Treatment_Models\IonExchangeModel\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdatsov\Documents\Programming\Params for HDMIX\Ver_20200615\IonExchangeModel\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B500B6D0-2C6F-4832-BDDD-7860F4E89FDE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75B4FBC-82B3-479A-8AB6-006A44077E51}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="-14115" windowWidth="21585" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2535" yWindow="405" windowWidth="15375" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="2" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>meq/g</t>
-  </si>
-  <si>
     <t>cm</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>RHOP</t>
   </si>
   <si>
-    <t>Qm</t>
-  </si>
-  <si>
     <t>mgN</t>
   </si>
   <si>
@@ -127,6 +121,12 @@
   </si>
   <si>
     <t>mg</t>
+  </si>
+  <si>
+    <t>Qf</t>
+  </si>
+  <si>
+    <t>meq/ml</t>
   </si>
 </sst>
 </file>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,29 +991,29 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2">
-        <v>1.5</v>
+        <v>0.58589999999999998</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>39.33</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>0.38</v>
@@ -1027,29 +1027,29 @@
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>10.199999999999999</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1060,29 +1060,29 @@
         <v>3.4500000000000003E-2</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1">
         <v>2.2000000000000001E-3</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1">
         <v>4.9999999999999998E-8</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1121,7 +1121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1178,7 +1178,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1195,7 +1195,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1212,7 +1212,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>